<commit_message>
Changed  formatting and updated archival page
</commit_message>
<xml_diff>
--- a/film-reviews.xlsx
+++ b/film-reviews.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="225">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch Date</t>
   </si>
   <si>
     <t xml:space="preserve">Tags</t>
@@ -686,9 +683,6 @@
     <t xml:space="preserve">https://en.wikipedia.org/wiki/HyperNormalisation</t>
   </si>
   <si>
-    <t xml:space="preserve">1/18/2020-1/22/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">Harold &amp; Kumar Go to White Castle</t>
   </si>
   <si>
@@ -785,9 +779,6 @@
     <t xml:space="preserve">https://en.wikipedia.org/wiki/Einstein_on_the_Beach#2010s</t>
   </si>
   <si>
-    <t xml:space="preserve">1/11/2020-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Climax</t>
   </si>
   <si>
@@ -837,6 +828,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://en.wikipedia.org/wiki/Carrie_(1976_film)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trolls World Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walt Dohrn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adventure, Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/Trolls_World_Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am not sure the creators know what genre is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anita: Speaking Truth to Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freida Lee Mock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.imdb.com/title/tt2481202/</t>
   </si>
   <si>
     <t xml:space="preserve">La Haine</t>
@@ -858,9 +873,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -953,7 +967,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -963,10 +977,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1060,20 +1070,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L45" activeCellId="0" sqref="L2:L45"/>
+      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="38.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,25 +1123,22 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2001</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>10</v>
@@ -1146,25 +1153,24 @@
         <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="3"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
@@ -1179,25 +1185,24 @@
         <v>9</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>6</v>
@@ -1209,28 +1214,27 @@
         <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>2</v>
@@ -1242,25 +1246,24 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1997</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>4</v>
@@ -1272,25 +1275,24 @@
         <v>4</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1971</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>3</v>
@@ -1302,25 +1304,24 @@
         <v>4</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2003</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>3</v>
@@ -1332,25 +1333,24 @@
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1986</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -1365,25 +1365,24 @@
         <v>3</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2006</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>2</v>
@@ -1395,25 +1394,24 @@
         <v>11</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="3"/>
+        <v>51</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>8</v>
@@ -1425,27 +1423,24 @@
         <v>5</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" s="3" t="n">
-        <v>43818</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>9</v>
@@ -1457,28 +1452,27 @@
         <v>2</v>
       </c>
       <c r="J12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1980</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>4</v>
@@ -1490,28 +1484,27 @@
         <v>7</v>
       </c>
       <c r="J13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1980</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>6</v>
@@ -1523,28 +1516,27 @@
         <v>9</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L14" s="3"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2003</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>1</v>
@@ -1553,25 +1545,24 @@
         <v>6</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L15" s="3"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1980</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>0</v>
@@ -1586,28 +1577,27 @@
         <v>7</v>
       </c>
       <c r="J16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="0" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2004</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>5</v>
@@ -1622,33 +1612,30 @@
         <v>11</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="L17" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="L17" s="3" t="n">
-        <v>43822</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>9</v>
@@ -1660,28 +1647,27 @@
         <v>8</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="0" t="s">
-        <v>60</v>
+        <v>93</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2007</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="E19" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>6</v>
@@ -1693,25 +1679,24 @@
         <v>11</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L19" s="3"/>
+        <v>98</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>102</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>0</v>
@@ -1723,27 +1708,24 @@
         <v>6</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" s="3" t="n">
-        <v>43822</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>7</v>
@@ -1755,25 +1737,24 @@
         <v>3</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L21" s="3"/>
+        <v>107</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1978</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="E22" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>1</v>
@@ -1785,25 +1766,24 @@
         <v>2</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="L22" s="3"/>
+        <v>111</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1983</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>11</v>
@@ -1815,25 +1795,24 @@
         <v>8</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" s="3"/>
+        <v>115</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1990</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>1</v>
@@ -1845,25 +1824,24 @@
         <v>8</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L24" s="3"/>
+        <v>120</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>125</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>2</v>
@@ -1875,25 +1853,24 @@
         <v>6</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L25" s="3"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>2003</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="E26" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>130</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
@@ -1908,25 +1885,24 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L26" s="3"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>134</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>5</v>
@@ -1938,25 +1914,24 @@
         <v>10</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="L27" s="3"/>
+        <v>134</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>139</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>4</v>
@@ -1971,25 +1946,24 @@
         <v>3</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L28" s="3"/>
+        <v>139</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>7</v>
@@ -2004,25 +1978,24 @@
         <v>8</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="L29" s="3"/>
+        <v>142</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1967</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>147</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>1</v>
@@ -2034,25 +2007,24 @@
         <v>9</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L30" s="3"/>
+        <v>147</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>2</v>
@@ -2064,28 +2036,27 @@
         <v>8</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L31" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>2006</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>157</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>9</v>
@@ -2097,28 +2068,27 @@
         <v>8</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>9</v>
@@ -2130,30 +2100,27 @@
         <v>7</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>2004</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>5</v>
@@ -2165,27 +2132,24 @@
         <v>10</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="L34" s="3" t="n">
-        <v>43941</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>173</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>8</v>
@@ -2197,25 +2161,24 @@
         <v>10</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="L35" s="3"/>
+        <v>172</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1982</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>178</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>6</v>
@@ -2227,28 +2190,27 @@
         <v>8</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="0" t="s">
-        <v>66</v>
+        <v>177</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1981</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>7</v>
@@ -2260,28 +2222,27 @@
         <v>8</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="0" t="s">
-        <v>28</v>
+        <v>181</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1973</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>7</v>
@@ -2293,30 +2254,27 @@
         <v>7</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L38" s="3" t="n">
-        <v>43856</v>
-      </c>
-      <c r="M38" s="0" t="s">
-        <v>154</v>
+        <v>185</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1977</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>11</v>
@@ -2328,51 +2286,47 @@
         <v>3</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="L39" s="3"/>
+        <v>189</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1976</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="J40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E40" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="M40" s="0" t="s">
-        <v>60</v>
+      <c r="L40" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>4</v>
@@ -2387,25 +2341,24 @@
         <v>3</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="L41" s="3"/>
+        <v>198</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>1</v>
@@ -2417,28 +2370,27 @@
         <v>9</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="0" t="s">
-        <v>28</v>
+        <v>202</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1982</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>6</v>
@@ -2450,28 +2402,27 @@
         <v>8</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="0" t="s">
-        <v>66</v>
+        <v>204</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1972</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>8</v>
@@ -2483,33 +2434,30 @@
         <v>8</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="L44" s="3" t="n">
-        <v>43870</v>
-      </c>
-      <c r="M44" s="0" t="s">
-        <v>66</v>
+        <v>208</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1976</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>7</v>
@@ -2521,9 +2469,69 @@
         <v>9</v>
       </c>
       <c r="J45" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="L45" s="3"/>
+      <c r="F46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2544,10 +2552,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="L2:L45 C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2559,23 +2567,23 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>218</v>
+        <v>222</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>219</v>
+      <c r="A4" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added zine, movie reviews, art section
</commit_message>
<xml_diff>
--- a/film-reviews.xlsx
+++ b/film-reviews.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="253">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -852,6 +852,90 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.imdb.com/title/tt2481202/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Peele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h 44m </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horror, Comedy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/Get_Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julia Ducournau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/Raw_(film)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thoroughbreds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cory Finley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h 32m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drama, Horror, Crime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/Thoroughbreds_(2017_film)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Truman Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drama, Existential Horror</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Wailing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peeping Tom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Adventures of Baron Munchausen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melancholia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mulholland Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children of Men</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inside Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Promises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/wiki/Eastern_Promises</t>
   </si>
   <si>
     <t xml:space="preserve">La Haine</t>
@@ -1070,13 +1154,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O52" activeCellId="0" sqref="O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.43"/>
@@ -2531,6 +2615,215 @@
       </c>
       <c r="J47" s="0" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1998</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>1966</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2555,7 +2848,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2567,23 +2860,23 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>221</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>